<commit_message>
Added extra logging variables.
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -105,10 +105,10 @@
     <t>X</t>
   </si>
   <si>
-    <t>sudo apt-get install sqlite3</t>
-  </si>
-  <si>
     <t>2015-06-05 / RPi2 / 64GB</t>
+  </si>
+  <si>
+    <t>sudo apt-get install sqlite3 php5-sqlite</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,7 +495,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E1" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C19" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
More instructions for Brian
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="179">
   <si>
     <t>sudo apt-get update; sudo apt-get upgrade</t>
   </si>
@@ -32,9 +32,6 @@
     <t>http://raspberrypihq.com/how-to-share-a-folder-with-a-windows-computer-from-a-raspberry-pi/</t>
   </si>
   <si>
-    <t>Setup samba share</t>
-  </si>
-  <si>
     <t>http://ubuntuforums.org/showthread.php?t=1723762</t>
   </si>
   <si>
@@ -44,9 +41,6 @@
     <t>setup hotspot</t>
   </si>
   <si>
-    <t>Set up RAM drive</t>
-  </si>
-  <si>
     <t>http://www.domoticz.com/wiki/Setting_up_a_RAM_drive_on_Raspberry_Pi</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
     <t>If a bash script gives the problem '$'\r': command not found</t>
   </si>
   <si>
-    <t>dos2unix /data/scripts/deletefiles</t>
-  </si>
-  <si>
     <t>*Need to install dos2unix</t>
   </si>
   <si>
@@ -515,9 +506,6 @@
     <t>turn_on_led.py</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>turn on led on startup</t>
   </si>
   <si>
@@ -525,6 +513,94 @@
   </si>
   <si>
     <t>see Folder Structure tab</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">sudo raspiconfig </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>and increase partition size  (first option)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Setup samba share for </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> folder</t>
+    </r>
+  </si>
+  <si>
+    <t>Set up RAM drive, 100MB?</t>
+  </si>
+  <si>
+    <r>
+      <t>dos2unix /data/scripts/</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>deletefiles</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">connect Rpi to vehicle, via diagnostics port (or custom harness if they remember to add that) </t>
+  </si>
+  <si>
+    <t>put can-test folder into /data/scripts</t>
+  </si>
+  <si>
+    <t>192.168.113.2XX</t>
+  </si>
+  <si>
+    <t>192.168.115.1</t>
+  </si>
+  <si>
+    <t>\\192.168.115.1\ in File Explorer</t>
+  </si>
+  <si>
+    <t>var?</t>
+  </si>
+  <si>
+    <t>website stuff goes here</t>
+  </si>
+  <si>
+    <t>LED:</t>
+  </si>
+  <si>
+    <t>Make sure green LED turns on when RPI is powered</t>
+  </si>
+  <si>
+    <t>Yellow LED turns on when RPI has booted and logged in.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +610,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,6 +674,13 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1626,13 +1709,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>553348</xdr:colOff>
-      <xdr:row>79</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>77234</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1714,13 +1797,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2124075</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1761,13 +1844,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>2152650</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2097,7 +2180,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,34 +2201,34 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="G1" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="H1" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="I1" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>79</v>
       </c>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
@@ -2159,7 +2242,7 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
       <c r="H2" s="23" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I2" s="24">
         <f>SUM(I3:I998)</f>
@@ -2177,29 +2260,29 @@
         <v>1</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F3" s="20">
         <v>2358</v>
       </c>
       <c r="G3" s="27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H3" s="28">
         <v>39.950000000000003</v>
       </c>
       <c r="I3" s="28">
-        <f t="shared" ref="I3:I21" si="0">H3*B3</f>
+        <f t="shared" ref="I3:I16" si="0">H3*B3</f>
         <v>39.950000000000003</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="K3" s="20"/>
       <c r="L3" s="20"/>
@@ -2213,19 +2296,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F4" s="20">
         <v>264</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H4" s="28">
         <v>9</v>
@@ -2235,33 +2318,33 @@
         <v>9</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="K4" s="20"/>
       <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="25">
-        <f t="shared" ref="A5:A21" si="1">A4+1</f>
+        <f t="shared" ref="A5:A16" si="1">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="26">
         <v>1</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D5" s="29" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F5" s="29">
         <v>814</v>
       </c>
       <c r="G5" s="29" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H5" s="30">
         <v>11.95</v>
@@ -2271,7 +2354,7 @@
         <v>11.95</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
@@ -2285,19 +2368,19 @@
         <v>1</v>
       </c>
       <c r="C6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="G6" s="29" t="s">
         <v>97</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>100</v>
       </c>
       <c r="H6" s="30">
         <v>50</v>
@@ -2307,7 +2390,7 @@
         <v>50</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
@@ -2321,19 +2404,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F7" s="20">
         <v>2083</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H7" s="31">
         <v>11.95</v>
@@ -2343,7 +2426,7 @@
         <v>11.95</v>
       </c>
       <c r="J7" s="32" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
@@ -2357,19 +2440,19 @@
         <v>1</v>
       </c>
       <c r="C8" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="F8" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="G8" s="35" t="s">
         <v>107</v>
-      </c>
-      <c r="E8" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="F8" s="34" t="s">
-        <v>109</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>110</v>
       </c>
       <c r="H8" s="30">
         <v>23</v>
@@ -2379,13 +2462,13 @@
         <v>23</v>
       </c>
       <c r="J8" s="32" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="L8" s="27" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -2397,19 +2480,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D9" s="33" t="s">
+      <c r="G9" s="33" t="s">
         <v>115</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>118</v>
       </c>
       <c r="H9" s="30">
         <v>20.6</v>
@@ -2419,7 +2502,7 @@
         <v>20.6</v>
       </c>
       <c r="J9" s="32" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
@@ -2433,13 +2516,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D10" s="33" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F10" s="33">
         <v>2310</v>
@@ -2453,7 +2536,7 @@
         <v>4.95</v>
       </c>
       <c r="J10" s="32" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K10" s="20"/>
       <c r="L10" s="20"/>
@@ -2467,13 +2550,13 @@
         <v>1</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D11" s="33" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E11" s="33" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F11" s="33">
         <v>2223</v>
@@ -2487,7 +2570,7 @@
         <v>2.5</v>
       </c>
       <c r="J11" s="32" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="K11" s="20"/>
       <c r="L11" s="20"/>
@@ -2501,19 +2584,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="29" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="G12" s="29" t="s">
         <v>127</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>130</v>
       </c>
       <c r="H12" s="30">
         <v>4.22</v>
@@ -2523,7 +2606,7 @@
         <v>4.22</v>
       </c>
       <c r="J12" s="32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="K12" s="20"/>
       <c r="L12" s="20"/>
@@ -2537,19 +2620,19 @@
         <v>1</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D13" s="29" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E13" s="29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G13" s="29" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="H13" s="30">
         <v>3.45</v>
@@ -2559,7 +2642,7 @@
         <v>3.45</v>
       </c>
       <c r="J13" s="32" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -2573,19 +2656,19 @@
         <v>2</v>
       </c>
       <c r="C14" s="20" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="E14" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F14" s="34" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="29" t="s">
+      <c r="G14" s="29" t="s">
         <v>137</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>139</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>140</v>
       </c>
       <c r="H14" s="30">
         <v>0.28000000000000003</v>
@@ -2595,7 +2678,7 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="J14" s="32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="K14" s="20"/>
       <c r="L14" s="20"/>
@@ -2609,19 +2692,19 @@
         <v>2</v>
       </c>
       <c r="C15" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="E15" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="F15" s="34" t="s">
+        <v>141</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>142</v>
-      </c>
-      <c r="D15" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G15" s="29" t="s">
-        <v>145</v>
       </c>
       <c r="H15" s="30">
         <v>0.1</v>
@@ -2631,7 +2714,7 @@
         <v>0.2</v>
       </c>
       <c r="J15" s="32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="K15" s="20"/>
       <c r="L15" s="20"/>
@@ -2646,16 +2729,16 @@
       </c>
       <c r="C16" s="20"/>
       <c r="D16" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="20" t="s">
         <v>147</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>150</v>
       </c>
       <c r="H16" s="31"/>
       <c r="I16" s="28">
@@ -2868,7 +2951,7 @@
   <dimension ref="A1:AS171"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2944,14 +3027,14 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
       <c r="I5" s="12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
@@ -3102,7 +3185,7 @@
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -3603,7 +3686,7 @@
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
       <c r="D19" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
@@ -3723,7 +3806,7 @@
       <c r="Z21" s="12"/>
       <c r="AA21" s="12"/>
       <c r="AB21" s="12" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="AC21" s="12"/>
       <c r="AD21" s="12"/>
@@ -4003,7 +4086,7 @@
       <c r="W27" s="12"/>
       <c r="X27" s="12"/>
       <c r="Y27" s="12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="Z27" s="12"/>
       <c r="AA27" s="12"/>
@@ -4222,7 +4305,7 @@
       <c r="G32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -4503,7 +4586,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="12"/>
       <c r="F38" s="12" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="G38" s="12"/>
       <c r="H38" s="12"/>
@@ -7593,10 +7676,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7610,21 +7693,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -7632,249 +7715,254 @@
         <v>0</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>170</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>163</v>
+      </c>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="E17" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" t="s">
-        <v>167</v>
-      </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>163</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
         <v>168</v>
       </c>
-      <c r="C21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>14</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B11" r:id="rId4"/>
-    <hyperlink ref="B6" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B13" r:id="rId7"/>
-    <hyperlink ref="B17" r:id="rId8"/>
-    <hyperlink ref="B8" r:id="rId9"/>
+    <hyperlink ref="B8" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B10" r:id="rId3"/>
+    <hyperlink ref="B12" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
+    <hyperlink ref="B13" r:id="rId6"/>
+    <hyperlink ref="B14" r:id="rId7"/>
+    <hyperlink ref="B18" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId9"/>
     <hyperlink ref="B1" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7885,10 +7973,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7900,181 +7988,214 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>42</v>
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>38</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="34" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
-        <v>63</v>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B35" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -8083,7 +8204,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8095,25 +8216,25 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="44"/>
       <c r="C3" s="44" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="44"/>
       <c r="C4" s="44"/>
       <c r="D4" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8164,14 +8285,14 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="44"/>
       <c r="C14" s="44" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="44"/>
       <c r="C15" s="44"/>
       <c r="D15" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8189,27 +8310,27 @@
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="44" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="44"/>
       <c r="C20" s="44" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="44"/>
       <c r="C21" s="44"/>
       <c r="D21" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="44"/>
       <c r="C22" s="44"/>
       <c r="E22" s="6" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -8222,17 +8343,20 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="44"/>
       <c r="C26" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="44"/>
+      <c r="D27" s="6" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="44"/>

</xml_diff>

<commit_message>
Julia learns what a string is. =/
</commit_message>
<xml_diff>
--- a/Commands.xlsx
+++ b/Commands.xlsx
@@ -576,9 +576,6 @@
     <t xml:space="preserve">connect Rpi to vehicle, via diagnostics port (or custom harness if they remember to add that) </t>
   </si>
   <si>
-    <t>put can-test folder into /data/scripts</t>
-  </si>
-  <si>
     <t>192.168.113.2XX</t>
   </si>
   <si>
@@ -601,6 +598,9 @@
   </si>
   <si>
     <t>Yellow LED turns on when RPI has booted and logged in.</t>
+  </si>
+  <si>
+    <t>put can-test folder into /data/scripts; bring up can on boot</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -775,7 +775,7 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -807,7 +807,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -819,10 +819,10 @@
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -834,16 +834,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -862,10 +862,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -7679,7 +7679,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7742,7 +7742,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -8120,7 +8120,7 @@
         <v>61</v>
       </c>
       <c r="B27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -8136,7 +8136,7 @@
         <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -8152,7 +8152,7 @@
         <v>52</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -8177,17 +8177,17 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -8343,7 +8343,7 @@
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
@@ -8355,7 +8355,7 @@
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="44"/>
       <c r="D27" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>